<commit_message>
Employee WorkLoad Edit Option Avaliable for Admins Now
</commit_message>
<xml_diff>
--- a/Dicionario de Classes Projeto Ponto.xlsx
+++ b/Dicionario de Classes Projeto Ponto.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26712"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26719"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E25747FF-E447-4EFF-8813-CD2DD79BDAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9C4CC96-1783-462F-995F-FD4444F8DD1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tb_funcionarios" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="68">
   <si>
     <t>tb_funcionarios</t>
   </si>
@@ -230,11 +230,33 @@
  deve começar o trabalho</t>
   </si>
   <si>
+    <t>Not Null</t>
+  </si>
+  <si>
     <t>horario_saida</t>
   </si>
   <si>
     <t>Horário que o funcionário
  deve finalizar o trabalho</t>
+  </si>
+  <si>
+    <t>Este Campo não pode ser nulo</t>
+  </si>
+  <si>
+    <t>horario_comeco
+_pausa</t>
+  </si>
+  <si>
+    <t>Horário que o funcionário
+ deve começar sua pausa</t>
+  </si>
+  <si>
+    <t>horario_fim
+_pausa</t>
+  </si>
+  <si>
+    <t>Horário que o funcionário
+ deve finalizar sua pausa</t>
   </si>
 </sst>
 </file>
@@ -420,83 +442,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -523,6 +488,69 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -855,194 +883,194 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="7"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="33"/>
     </row>
     <row r="3" spans="2:7">
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="30"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="10"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="30"/>
     </row>
     <row r="6" spans="2:7" ht="15" customHeight="1">
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="13"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="26"/>
     </row>
     <row r="7" spans="2:7" ht="30.75">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="60.75">
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="30" customHeight="1">
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>50</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="19" t="s">
+      <c r="G9" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="30" customHeight="1">
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>11</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="6" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="30" customHeight="1">
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>50</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="30" customHeight="1">
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>30</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="2:7" ht="76.5">
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4" t="s">
+      <c r="E13" s="3"/>
+      <c r="F13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1075,101 +1103,101 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="33"/>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="28" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="10"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="30"/>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="10"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="30"/>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="36"/>
     </row>
     <row r="8" spans="2:7" ht="47.25" customHeight="1">
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="18" t="s">
+      <c r="F8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="5" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="78" customHeight="1">
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="20" t="s">
         <v>40</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -1183,20 +1211,20 @@
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="2:7" ht="76.5">
-      <c r="B11" s="38" t="s">
+      <c r="B11" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4" t="s">
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1230,104 +1258,104 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="33"/>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="27" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="10"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="30"/>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="10"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="30"/>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="39"/>
     </row>
     <row r="8" spans="2:7" ht="60.75">
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="23" t="s">
+      <c r="F8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="7" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="78.75" customHeight="1">
-      <c r="B9" s="34" t="s">
+      <c r="B9" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="30" customHeight="1">
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="6" t="s">
         <v>51</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -1339,27 +1367,27 @@
       <c r="F10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="30" customHeight="1">
-      <c r="B11" s="34" t="s">
+      <c r="B11" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>30</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1377,10 +1405,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B998643B-5E86-4EA9-B17A-7A2C9DE33962}">
-  <dimension ref="B2:G11"/>
+  <dimension ref="B2:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1393,124 +1421,160 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="33"/>
     </row>
     <row r="4" spans="2:7">
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="10"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="30"/>
     </row>
     <row r="6" spans="2:7">
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="10"/>
+      <c r="C6" s="28"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="30"/>
     </row>
     <row r="7" spans="2:7">
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="26"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
+      <c r="G7" s="42"/>
     </row>
     <row r="8" spans="2:7" ht="60.75">
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="27" t="s">
+      <c r="D8" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="27" t="s">
+      <c r="F8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="27" t="s">
+      <c r="G8" s="8" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="82.5" customHeight="1">
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4" t="s">
+      <c r="E9" s="3"/>
+      <c r="F9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="30" customHeight="1">
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="6" t="s">
         <v>59</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>42</v>
       </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="19"/>
+      <c r="F10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="11" spans="2:7" ht="30" customHeight="1">
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="G11" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="30.75">
+      <c r="B12" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="3"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="6"/>
+    </row>
+    <row r="13" spans="2:7" ht="30.75">
+      <c r="B13" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>